<commit_message>
Update Dhruva FM order
</commit_message>
<xml_diff>
--- a/BOM_STS1_Sidepanels.xlsx
+++ b/BOM_STS1_Sidepanels.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="89">
   <si>
     <t>ID</t>
   </si>
@@ -44,15 +44,9 @@
     <t>22R</t>
   </si>
   <si>
-    <t>C51,C61,C11,C62,C12,C52</t>
-  </si>
-  <si>
     <t>C_0805_2012Metric</t>
   </si>
   <si>
-    <t>22u</t>
-  </si>
-  <si>
     <t>TH1</t>
   </si>
   <si>
@@ -80,27 +74,18 @@
     <t>SMM4F5.0</t>
   </si>
   <si>
-    <t>MPPT2,MPPT1</t>
-  </si>
-  <si>
     <t>TSSOP-8_4.4x3mm_P0.65mm</t>
   </si>
   <si>
     <t>SPV1040TTR</t>
   </si>
   <si>
-    <t>R22,R42,R21,R32,R41,R71,R31</t>
-  </si>
-  <si>
     <t>R_0603_1608Metric</t>
   </si>
   <si>
     <t>1k</t>
   </si>
   <si>
-    <t>D12,D11</t>
-  </si>
-  <si>
     <t>D_SOD-123F</t>
   </si>
   <si>
@@ -113,57 +98,30 @@
     <t>3k</t>
   </si>
   <si>
-    <t>R12,R11</t>
-  </si>
-  <si>
     <t>R_0805_2012Metric</t>
   </si>
   <si>
     <t>10m</t>
   </si>
   <si>
-    <t>U12,U11</t>
-  </si>
-  <si>
     <t>SOT-23-5</t>
   </si>
   <si>
     <t>INA180A4</t>
   </si>
   <si>
-    <t>R52,R51</t>
-  </si>
-  <si>
     <t>220m</t>
   </si>
   <si>
-    <t>C31,C32,C22,C21</t>
-  </si>
-  <si>
     <t>C_0603_1608Metric</t>
   </si>
   <si>
     <t>1n</t>
   </si>
   <si>
-    <t>C42,C41</t>
-  </si>
-  <si>
     <t>1u</t>
   </si>
   <si>
-    <t>R62</t>
-  </si>
-  <si>
-    <t>1M</t>
-  </si>
-  <si>
-    <t>R72</t>
-  </si>
-  <si>
-    <t>330k</t>
-  </si>
-  <si>
     <t>J1</t>
   </si>
   <si>
@@ -194,15 +152,9 @@
     <t>Conn_01x08</t>
   </si>
   <si>
-    <t>C21,C31,C22,C32</t>
-  </si>
-  <si>
     <t>L1,L2</t>
   </si>
   <si>
-    <t>C11,C61,C41,C12,C62,C42</t>
-  </si>
-  <si>
     <t>RU1,RU2</t>
   </si>
   <si>
@@ -224,24 +176,12 @@
     <t>501461-0491</t>
   </si>
   <si>
-    <t>R62,R61</t>
-  </si>
-  <si>
-    <t>R22,R31,R21,R41,R32,R42</t>
-  </si>
-  <si>
-    <t>C52,C1,C51</t>
-  </si>
-  <si>
     <t>R11,R12</t>
   </si>
   <si>
     <t>R51,R52</t>
   </si>
   <si>
-    <t>R72,R71</t>
-  </si>
-  <si>
     <t>IC1</t>
   </si>
   <si>
@@ -251,39 +191,21 @@
     <t>TMP112AQDRLRQ1</t>
   </si>
   <si>
-    <t>R71</t>
-  </si>
-  <si>
     <t>edu_con1,cam1</t>
   </si>
   <si>
     <t>54548-2271</t>
   </si>
   <si>
-    <t>R31,R21,R41</t>
-  </si>
-  <si>
     <t>C1,C51</t>
   </si>
   <si>
-    <t>C11,C61,C41</t>
-  </si>
-  <si>
-    <t>RU2,RU1</t>
-  </si>
-  <si>
     <t>D21</t>
   </si>
   <si>
     <t>L1</t>
   </si>
   <si>
-    <t>C21</t>
-  </si>
-  <si>
-    <t>100n</t>
-  </si>
-  <si>
     <t>SAMTEC_ZF5S-16-01-T-WT</t>
   </si>
   <si>
@@ -293,9 +215,6 @@
     <t>U11</t>
   </si>
   <si>
-    <t>C31</t>
-  </si>
-  <si>
     <t>MPPT1</t>
   </si>
   <si>
@@ -311,27 +230,12 @@
     <t>C21,C31</t>
   </si>
   <si>
-    <t>R41,R31,R21</t>
-  </si>
-  <si>
     <t>edu_con2,cam2</t>
   </si>
   <si>
-    <t>C11,C41,C61</t>
-  </si>
-  <si>
     <t>Count</t>
   </si>
   <si>
-    <t>R71 falsch?</t>
-  </si>
-  <si>
-    <t>nicht bestellt</t>
-  </si>
-  <si>
-    <t>10V oder 6.3V</t>
-  </si>
-  <si>
     <t>Rechnung raussuchen, STS1 - B23-191</t>
   </si>
   <si>
@@ -339,6 +243,48 @@
   </si>
   <si>
     <t>im HQ</t>
+  </si>
+  <si>
+    <t>22u 10V</t>
+  </si>
+  <si>
+    <t>22u 6.3V</t>
+  </si>
+  <si>
+    <t>R21,R22,R31,R32,R41,R42,R71,R72</t>
+  </si>
+  <si>
+    <t>R61,R62</t>
+  </si>
+  <si>
+    <t>C51,C52</t>
+  </si>
+  <si>
+    <t>C41,C42</t>
+  </si>
+  <si>
+    <t>C11,C12,C61,C62</t>
+  </si>
+  <si>
+    <t>C11,C61</t>
+  </si>
+  <si>
+    <t>C41</t>
+  </si>
+  <si>
+    <t>C1,C51,C52</t>
+  </si>
+  <si>
+    <t>U11,U12</t>
+  </si>
+  <si>
+    <t>C21,C22,C31,C32</t>
+  </si>
+  <si>
+    <t>R21,R31,R41,R71</t>
+  </si>
+  <si>
+    <t>Digikey</t>
   </si>
 </sst>
 </file>
@@ -725,16 +671,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G19"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="45.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="21.85546875" bestFit="1" customWidth="1"/>
@@ -751,7 +697,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>100</v>
+        <v>71</v>
       </c>
       <c r="E1" t="s">
         <v>4</v>
@@ -780,37 +726,34 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C3" t="s">
         <v>8</v>
       </c>
-      <c r="C3" t="s">
-        <v>9</v>
-      </c>
       <c r="D3">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="E3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" s="3"/>
-      <c r="G3" t="s">
-        <v>103</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="F3" s="1"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>81</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D4">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E4" t="s">
-        <v>13</v>
+        <v>76</v>
       </c>
       <c r="F4" s="1"/>
     </row>
@@ -819,16 +762,16 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D5">
         <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="F5" s="1"/>
     </row>
@@ -837,16 +780,16 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C6" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="D6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E6" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="F6" s="1"/>
     </row>
@@ -855,41 +798,38 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C7" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="D7">
         <v>2</v>
       </c>
       <c r="E7" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="F7" s="1"/>
-      <c r="G7" t="s">
-        <v>105</v>
-      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>23</v>
+        <v>48</v>
       </c>
       <c r="C8" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="D8">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="E8" t="s">
-        <v>25</v>
-      </c>
-      <c r="F8" s="3"/>
+        <v>19</v>
+      </c>
+      <c r="F8" s="1"/>
       <c r="G8" t="s">
-        <v>101</v>
+        <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -897,16 +837,16 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>26</v>
+        <v>77</v>
       </c>
       <c r="C9" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="D9">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="E9" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="F9" s="1"/>
     </row>
@@ -915,34 +855,34 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>29</v>
+        <v>47</v>
       </c>
       <c r="C10" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E10" t="s">
-        <v>30</v>
-      </c>
-      <c r="F10" s="2"/>
+        <v>23</v>
+      </c>
+      <c r="F10" s="1"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>31</v>
+        <v>78</v>
       </c>
       <c r="C11" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="D11">
         <v>2</v>
       </c>
       <c r="E11" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="F11" s="1"/>
     </row>
@@ -951,16 +891,16 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>34</v>
+        <v>52</v>
       </c>
       <c r="C12" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="D12">
         <v>2</v>
       </c>
       <c r="E12" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="F12" s="1"/>
     </row>
@@ -969,16 +909,16 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>37</v>
+        <v>85</v>
       </c>
       <c r="C13" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D13">
         <v>2</v>
       </c>
       <c r="E13" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="F13" s="1"/>
     </row>
@@ -987,16 +927,16 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>39</v>
+        <v>53</v>
       </c>
       <c r="C14" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="D14">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E14" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="F14" s="1"/>
     </row>
@@ -1005,16 +945,16 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>42</v>
+        <v>86</v>
       </c>
       <c r="C15" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="D15">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E15" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="F15" s="1"/>
     </row>
@@ -1023,16 +963,16 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>44</v>
+        <v>79</v>
       </c>
       <c r="C16" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="D16">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E16" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="F16" s="1"/>
     </row>
@@ -1041,59 +981,38 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="C17" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="D17">
         <v>1</v>
       </c>
       <c r="E17" t="s">
-        <v>47</v>
-      </c>
-      <c r="F17" s="2"/>
-      <c r="G17" t="s">
-        <v>102</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="F17" s="1"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="C18" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="D18">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E18" t="s">
-        <v>50</v>
-      </c>
-      <c r="F18" s="1"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>18</v>
-      </c>
-      <c r="B19" t="s">
-        <v>51</v>
-      </c>
-      <c r="C19" t="s">
-        <v>52</v>
-      </c>
-      <c r="D19">
-        <v>2</v>
-      </c>
-      <c r="E19" t="s">
-        <v>53</v>
-      </c>
-      <c r="F19" s="2"/>
-      <c r="G19" t="s">
-        <v>102</v>
+        <v>39</v>
+      </c>
+      <c r="F18" s="2"/>
+      <c r="G18" t="s">
+        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -1106,13 +1025,13 @@
   <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:G2"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="45.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.5703125" bestFit="1" customWidth="1"/>
@@ -1140,20 +1059,20 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="C2" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="D2">
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="F2" s="3"/>
       <c r="G2" t="s">
-        <v>106</v>
+        <v>74</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -1161,16 +1080,16 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="C3" t="s">
-        <v>49</v>
+        <v>35</v>
       </c>
       <c r="D3">
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="F3" s="1"/>
     </row>
@@ -1179,16 +1098,16 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>58</v>
+        <v>86</v>
       </c>
       <c r="C4" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="D4">
         <v>4</v>
       </c>
       <c r="E4" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="F4" s="1"/>
     </row>
@@ -1197,20 +1116,20 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>59</v>
+        <v>44</v>
       </c>
       <c r="C5" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="D5">
         <v>2</v>
       </c>
       <c r="E5" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" t="s">
-        <v>102</v>
+        <v>88</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -1218,58 +1137,52 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="C6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D6">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="E6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F6" s="3"/>
-      <c r="G6" t="s">
-        <v>103</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="F6" s="1"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>61</v>
+        <v>81</v>
       </c>
       <c r="C7" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="D7">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E7" t="s">
-        <v>62</v>
+        <v>76</v>
       </c>
       <c r="F7" s="1"/>
-      <c r="G7" t="s">
-        <v>104</v>
-      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>63</v>
+        <v>45</v>
       </c>
       <c r="C8" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="D8">
         <v>2</v>
       </c>
       <c r="E8" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="F8" s="1"/>
     </row>
@@ -1278,37 +1191,34 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>64</v>
+        <v>47</v>
       </c>
       <c r="C9" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D9">
         <v>2</v>
       </c>
       <c r="E9" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F9" s="1"/>
-      <c r="G9" t="s">
-        <v>105</v>
-      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>65</v>
+        <v>48</v>
       </c>
       <c r="C10" t="s">
-        <v>66</v>
+        <v>18</v>
       </c>
       <c r="D10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E10" t="s">
-        <v>67</v>
+        <v>19</v>
       </c>
       <c r="F10" s="1"/>
     </row>
@@ -1317,31 +1227,34 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>68</v>
+        <v>49</v>
       </c>
       <c r="C11" t="s">
-        <v>24</v>
+        <v>50</v>
       </c>
       <c r="D11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E11" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="F11" s="1"/>
+      <c r="G11" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>69</v>
+        <v>78</v>
       </c>
       <c r="C12" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="D12">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="E12" t="s">
         <v>25</v>
@@ -1353,16 +1266,16 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>17</v>
+        <v>77</v>
       </c>
       <c r="C13" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D13">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="E13" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="F13" s="1"/>
     </row>
@@ -1371,16 +1284,16 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>34</v>
+        <v>15</v>
       </c>
       <c r="C14" t="s">
-        <v>35</v>
+        <v>16</v>
       </c>
       <c r="D14">
         <v>2</v>
       </c>
       <c r="E14" t="s">
-        <v>36</v>
+        <v>17</v>
       </c>
       <c r="F14" s="1"/>
     </row>
@@ -1389,16 +1302,16 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>70</v>
+        <v>85</v>
       </c>
       <c r="C15" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="D15">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E15" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="F15" s="1"/>
     </row>
@@ -1407,91 +1320,88 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>71</v>
+        <v>84</v>
       </c>
       <c r="C16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D16">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E16" t="s">
         <v>33</v>
       </c>
       <c r="F16" s="1"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>72</v>
+        <v>52</v>
       </c>
       <c r="C17" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="D17">
         <v>2</v>
       </c>
       <c r="E17" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="F17" s="1"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>11</v>
+        <v>53</v>
       </c>
       <c r="C18" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="D18">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E18" t="s">
-        <v>13</v>
+        <v>30</v>
       </c>
       <c r="F18" s="1"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>73</v>
+        <v>9</v>
       </c>
       <c r="C19" t="s">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="D19">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E19" t="s">
-        <v>47</v>
-      </c>
-      <c r="F19" s="2"/>
-      <c r="G19" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+      <c r="F19" s="1"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>74</v>
+        <v>54</v>
       </c>
       <c r="C20" t="s">
-        <v>75</v>
+        <v>55</v>
       </c>
       <c r="D20">
         <v>1</v>
       </c>
       <c r="E20" t="s">
-        <v>76</v>
+        <v>56</v>
       </c>
       <c r="F20" s="1"/>
     </row>
@@ -1505,13 +1415,13 @@
   <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:G2"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="45.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.5703125" bestFit="1" customWidth="1"/>
@@ -1539,20 +1449,20 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="C2" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="D2">
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="F2" s="3"/>
       <c r="G2" t="s">
-        <v>106</v>
+        <v>74</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -1560,16 +1470,16 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="C3" t="s">
-        <v>49</v>
+        <v>35</v>
       </c>
       <c r="D3">
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="F3" s="1"/>
     </row>
@@ -1578,16 +1488,16 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>58</v>
+        <v>86</v>
       </c>
       <c r="C4" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="D4">
         <v>4</v>
       </c>
       <c r="E4" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="F4" s="1"/>
     </row>
@@ -1596,20 +1506,20 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>59</v>
+        <v>44</v>
       </c>
       <c r="C5" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="D5">
         <v>2</v>
       </c>
       <c r="E5" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" t="s">
-        <v>102</v>
+        <v>88</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -1617,130 +1527,124 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="C6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D6">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="E6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F6" s="3"/>
-      <c r="G6" t="s">
-        <v>103</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="F6" s="1"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>61</v>
+        <v>81</v>
       </c>
       <c r="C7" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="D7">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E7" t="s">
-        <v>62</v>
+        <v>76</v>
       </c>
       <c r="F7" s="1"/>
-      <c r="G7" t="s">
-        <v>104</v>
-      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>63</v>
+        <v>45</v>
       </c>
       <c r="C8" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="D8">
         <v>2</v>
       </c>
       <c r="E8" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="F8" s="1"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>64</v>
+        <v>47</v>
       </c>
       <c r="C9" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D9">
         <v>2</v>
       </c>
       <c r="E9" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F9" s="1"/>
-      <c r="G9" t="s">
-        <v>105</v>
-      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>65</v>
+        <v>48</v>
       </c>
       <c r="C10" t="s">
-        <v>66</v>
+        <v>18</v>
       </c>
       <c r="D10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E10" t="s">
-        <v>67</v>
+        <v>19</v>
       </c>
       <c r="F10" s="1"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>68</v>
+        <v>49</v>
       </c>
       <c r="C11" t="s">
-        <v>24</v>
+        <v>50</v>
       </c>
       <c r="D11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E11" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="F11" s="1"/>
+      <c r="G11" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>69</v>
+        <v>78</v>
       </c>
       <c r="C12" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="D12">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="E12" t="s">
         <v>25</v>
@@ -1749,148 +1653,145 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>17</v>
+        <v>77</v>
       </c>
       <c r="C13" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D13">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="E13" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="F13" s="1"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>34</v>
+        <v>15</v>
       </c>
       <c r="C14" t="s">
-        <v>35</v>
+        <v>16</v>
       </c>
       <c r="D14">
         <v>2</v>
       </c>
       <c r="E14" t="s">
-        <v>36</v>
+        <v>17</v>
       </c>
       <c r="F14" s="1"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>70</v>
+        <v>85</v>
       </c>
       <c r="C15" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="D15">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E15" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="F15" s="1"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>71</v>
+        <v>84</v>
       </c>
       <c r="C16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D16">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E16" t="s">
         <v>33</v>
       </c>
       <c r="F16" s="1"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
+        <v>52</v>
+      </c>
+      <c r="C17" t="s">
+        <v>26</v>
+      </c>
+      <c r="D17">
+        <v>2</v>
+      </c>
+      <c r="E17" t="s">
+        <v>27</v>
+      </c>
+      <c r="F17" s="1"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18">
         <v>16</v>
       </c>
-      <c r="B17" t="s">
-        <v>72</v>
-      </c>
-      <c r="C17" t="s">
-        <v>32</v>
-      </c>
-      <c r="D17">
-        <v>2</v>
-      </c>
-      <c r="E17" t="s">
-        <v>38</v>
-      </c>
-      <c r="F17" s="1"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18">
+      <c r="B18" t="s">
+        <v>53</v>
+      </c>
+      <c r="C18" t="s">
+        <v>26</v>
+      </c>
+      <c r="D18">
+        <v>2</v>
+      </c>
+      <c r="E18" t="s">
+        <v>30</v>
+      </c>
+      <c r="F18" s="1"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19">
         <v>17</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B19" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19" t="s">
+        <v>10</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19" t="s">
         <v>11</v>
       </c>
-      <c r="C18" t="s">
-        <v>12</v>
-      </c>
-      <c r="D18">
-        <v>1</v>
-      </c>
-      <c r="E18" t="s">
-        <v>13</v>
-      </c>
-      <c r="F18" s="1"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19">
+      <c r="F19" s="1"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20">
         <v>18</v>
       </c>
-      <c r="B19" t="s">
-        <v>73</v>
-      </c>
-      <c r="C19" t="s">
-        <v>24</v>
-      </c>
-      <c r="D19">
-        <v>2</v>
-      </c>
-      <c r="E19" t="s">
-        <v>47</v>
-      </c>
-      <c r="F19" s="2"/>
-      <c r="G19" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>19</v>
-      </c>
       <c r="B20" t="s">
-        <v>74</v>
+        <v>54</v>
       </c>
       <c r="C20" t="s">
-        <v>75</v>
+        <v>55</v>
       </c>
       <c r="D20">
         <v>1</v>
       </c>
       <c r="E20" t="s">
-        <v>76</v>
+        <v>56</v>
       </c>
       <c r="F20" s="1"/>
     </row>
@@ -1901,16 +1802,16 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:G2"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="45.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.5703125" bestFit="1" customWidth="1"/>
@@ -1938,20 +1839,20 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="C2" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="D2">
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="F2" s="3"/>
       <c r="G2" t="s">
-        <v>106</v>
+        <v>74</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -1959,20 +1860,20 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>77</v>
-      </c>
-      <c r="C3" t="s">
-        <v>24</v>
+        <v>57</v>
+      </c>
+      <c r="C3" s="4">
+        <v>545482271</v>
       </c>
       <c r="D3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E3" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" t="s">
-        <v>102</v>
+        <v>88</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -1980,37 +1881,34 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>78</v>
-      </c>
-      <c r="C4" s="4">
-        <v>545482271</v>
+        <v>87</v>
+      </c>
+      <c r="C4" t="s">
+        <v>20</v>
       </c>
       <c r="D4">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E4" t="s">
-        <v>79</v>
-      </c>
-      <c r="F4" s="2"/>
-      <c r="G4" t="s">
-        <v>102</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="F4" s="1"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>80</v>
+        <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="D5">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="F5" s="1"/>
     </row>
@@ -2019,16 +1917,16 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>49</v>
       </c>
       <c r="C6" t="s">
-        <v>12</v>
+        <v>50</v>
       </c>
       <c r="D6">
         <v>1</v>
       </c>
       <c r="E6" t="s">
-        <v>13</v>
+        <v>51</v>
       </c>
       <c r="F6" s="1"/>
     </row>
@@ -2037,16 +1935,16 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="C7" t="s">
-        <v>66</v>
+        <v>31</v>
       </c>
       <c r="D7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E7" t="s">
-        <v>67</v>
+        <v>33</v>
       </c>
       <c r="F7" s="1"/>
     </row>
@@ -2055,16 +1953,16 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>81</v>
+        <v>54</v>
       </c>
       <c r="C8" t="s">
-        <v>40</v>
+        <v>55</v>
       </c>
       <c r="D8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E8" t="s">
-        <v>43</v>
+        <v>56</v>
       </c>
       <c r="F8" s="1"/>
     </row>
@@ -2073,16 +1971,16 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>74</v>
+        <v>83</v>
       </c>
       <c r="C9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9" t="s">
         <v>75</v>
-      </c>
-      <c r="D9">
-        <v>1</v>
-      </c>
-      <c r="E9" t="s">
-        <v>76</v>
       </c>
       <c r="F9" s="1"/>
     </row>
@@ -2094,38 +1992,35 @@
         <v>82</v>
       </c>
       <c r="C10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D10">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E10" t="s">
-        <v>10</v>
-      </c>
-      <c r="F10" s="3"/>
-      <c r="G10" t="s">
-        <v>103</v>
-      </c>
+        <v>76</v>
+      </c>
+      <c r="F10" s="1"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>83</v>
+        <v>45</v>
       </c>
       <c r="C11" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="D11">
         <v>2</v>
       </c>
       <c r="E11" t="s">
-        <v>62</v>
+        <v>46</v>
       </c>
       <c r="F11" s="1"/>
       <c r="G11" t="s">
-        <v>104</v>
+        <v>72</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -2133,16 +2028,16 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>84</v>
+        <v>60</v>
       </c>
       <c r="C12" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D12">
         <v>1</v>
       </c>
       <c r="E12" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F12" s="1"/>
     </row>
@@ -2151,20 +2046,20 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>85</v>
+        <v>61</v>
       </c>
       <c r="C13" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="D13">
         <v>1</v>
       </c>
       <c r="E13" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="F13" s="2"/>
       <c r="G13" t="s">
-        <v>102</v>
+        <v>88</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -2172,34 +2067,34 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>86</v>
+        <v>34</v>
       </c>
       <c r="C14" t="s">
-        <v>40</v>
+        <v>62</v>
       </c>
       <c r="D14">
         <v>1</v>
       </c>
       <c r="E14" t="s">
-        <v>87</v>
-      </c>
-      <c r="F14" s="2"/>
+        <v>63</v>
+      </c>
+      <c r="F14" s="1"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>48</v>
+        <v>64</v>
       </c>
       <c r="C15" t="s">
-        <v>88</v>
+        <v>28</v>
       </c>
       <c r="D15">
         <v>1</v>
       </c>
       <c r="E15" t="s">
-        <v>89</v>
+        <v>29</v>
       </c>
       <c r="F15" s="1"/>
     </row>
@@ -2208,16 +2103,16 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>90</v>
+        <v>24</v>
       </c>
       <c r="C16" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="D16">
         <v>1</v>
       </c>
       <c r="E16" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="F16" s="1"/>
     </row>
@@ -2226,16 +2121,16 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>29</v>
+        <v>69</v>
       </c>
       <c r="C17" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="D17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E17" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="F17" s="1"/>
     </row>
@@ -2244,55 +2139,55 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>91</v>
+        <v>65</v>
       </c>
       <c r="C18" t="s">
-        <v>40</v>
+        <v>18</v>
       </c>
       <c r="D18">
         <v>1</v>
       </c>
       <c r="E18" t="s">
-        <v>41</v>
+        <v>19</v>
       </c>
       <c r="F18" s="1"/>
+      <c r="G18" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>92</v>
+        <v>66</v>
       </c>
       <c r="C19" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="D19">
         <v>1</v>
       </c>
       <c r="E19" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="F19" s="1"/>
-      <c r="G19" t="s">
-        <v>105</v>
-      </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>93</v>
+        <v>67</v>
       </c>
       <c r="C20" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="D20">
         <v>1</v>
       </c>
       <c r="E20" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="F20" s="1"/>
     </row>
@@ -2301,36 +2196,18 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>94</v>
+        <v>68</v>
       </c>
       <c r="C21" t="s">
+        <v>26</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+      <c r="E21" t="s">
         <v>27</v>
       </c>
-      <c r="D21">
-        <v>1</v>
-      </c>
-      <c r="E21" t="s">
-        <v>28</v>
-      </c>
       <c r="F21" s="1"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>21</v>
-      </c>
-      <c r="B22" t="s">
-        <v>95</v>
-      </c>
-      <c r="C22" t="s">
-        <v>32</v>
-      </c>
-      <c r="D22">
-        <v>1</v>
-      </c>
-      <c r="E22" t="s">
-        <v>33</v>
-      </c>
-      <c r="F22" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -2342,13 +2219,13 @@
   <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:G2"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="45.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.5703125" bestFit="1" customWidth="1"/>
@@ -2376,20 +2253,20 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="C2" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="D2">
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="F2" s="3"/>
       <c r="G2" t="s">
-        <v>106</v>
+        <v>74</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -2397,16 +2274,16 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>81</v>
+        <v>59</v>
       </c>
       <c r="C3" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="D3">
         <v>2</v>
       </c>
       <c r="E3" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="F3" s="1"/>
     </row>
@@ -2415,16 +2292,16 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>74</v>
+        <v>54</v>
       </c>
       <c r="C4" t="s">
-        <v>75</v>
+        <v>55</v>
       </c>
       <c r="D4">
         <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>76</v>
+        <v>56</v>
       </c>
       <c r="F4" s="1"/>
     </row>
@@ -2433,16 +2310,16 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>96</v>
+        <v>69</v>
       </c>
       <c r="C5" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="D5">
         <v>2</v>
       </c>
       <c r="E5" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="F5" s="1"/>
     </row>
@@ -2451,20 +2328,20 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>92</v>
+        <v>65</v>
       </c>
       <c r="C6" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D6">
         <v>1</v>
       </c>
       <c r="E6" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="F6" s="1"/>
       <c r="G6" t="s">
-        <v>105</v>
+        <v>73</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -2472,37 +2349,34 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>77</v>
+        <v>60</v>
       </c>
       <c r="C7" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="D7">
         <v>1</v>
       </c>
       <c r="E7" t="s">
-        <v>47</v>
-      </c>
-      <c r="F7" s="2"/>
-      <c r="G7" t="s">
-        <v>102</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="F7" s="1"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>84</v>
+        <v>66</v>
       </c>
       <c r="C8" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="D8">
         <v>1</v>
       </c>
       <c r="E8" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="F8" s="1"/>
     </row>
@@ -2511,16 +2385,16 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>93</v>
+        <v>24</v>
       </c>
       <c r="C9" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="D9">
         <v>1</v>
       </c>
       <c r="E9" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="F9" s="1"/>
     </row>
@@ -2529,16 +2403,16 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>29</v>
+        <v>87</v>
       </c>
       <c r="C10" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="D10">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E10" t="s">
-        <v>45</v>
+        <v>21</v>
       </c>
       <c r="F10" s="1"/>
     </row>
@@ -2547,38 +2421,41 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>97</v>
+        <v>61</v>
       </c>
       <c r="C11" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="D11">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E11" t="s">
-        <v>25</v>
-      </c>
-      <c r="F11" s="1"/>
+        <v>39</v>
+      </c>
+      <c r="F11" s="2"/>
+      <c r="G11" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>85</v>
+        <v>45</v>
       </c>
       <c r="C12" t="s">
-        <v>52</v>
+        <v>20</v>
       </c>
       <c r="D12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E12" t="s">
-        <v>53</v>
-      </c>
-      <c r="F12" s="2"/>
+        <v>46</v>
+      </c>
+      <c r="F12" s="1"/>
       <c r="G12" t="s">
-        <v>102</v>
+        <v>72</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -2586,37 +2463,34 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>83</v>
+        <v>68</v>
       </c>
       <c r="C13" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D13">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E13" t="s">
-        <v>62</v>
+        <v>27</v>
       </c>
       <c r="F13" s="1"/>
-      <c r="G13" t="s">
-        <v>104</v>
-      </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>95</v>
+        <v>34</v>
       </c>
       <c r="C14" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="D14">
         <v>1</v>
       </c>
       <c r="E14" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="F14" s="1"/>
     </row>
@@ -2625,130 +2499,127 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>48</v>
-      </c>
-      <c r="C15" t="s">
-        <v>49</v>
+        <v>70</v>
+      </c>
+      <c r="C15" s="4">
+        <v>545482271</v>
       </c>
       <c r="D15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E15" t="s">
-        <v>57</v>
-      </c>
-      <c r="F15" s="1"/>
+        <v>58</v>
+      </c>
+      <c r="F15" s="2"/>
+      <c r="G15" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>98</v>
-      </c>
-      <c r="C16" s="4">
-        <v>545482271</v>
+        <v>49</v>
+      </c>
+      <c r="C16" t="s">
+        <v>50</v>
       </c>
       <c r="D16">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E16" t="s">
-        <v>79</v>
-      </c>
-      <c r="F16" s="2"/>
-      <c r="G16" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+      <c r="F16" s="1"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>65</v>
+        <v>83</v>
       </c>
       <c r="C17" t="s">
-        <v>66</v>
+        <v>8</v>
       </c>
       <c r="D17">
         <v>1</v>
       </c>
       <c r="E17" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="F17" s="1"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>99</v>
+        <v>82</v>
       </c>
       <c r="C18" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D18">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E18" t="s">
-        <v>10</v>
-      </c>
-      <c r="F18" s="3"/>
-      <c r="G18" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+      <c r="F18" s="1"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19" t="s">
+        <v>10</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19" t="s">
         <v>11</v>
       </c>
-      <c r="C19" t="s">
-        <v>12</v>
-      </c>
-      <c r="D19">
-        <v>1</v>
-      </c>
-      <c r="E19" t="s">
-        <v>13</v>
-      </c>
       <c r="F19" s="1"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>90</v>
+        <v>64</v>
       </c>
       <c r="C20" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="D20">
         <v>1</v>
       </c>
       <c r="E20" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="F20" s="1"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>94</v>
+        <v>67</v>
       </c>
       <c r="C21" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="D21">
         <v>1</v>
       </c>
       <c r="E21" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="F21" s="1"/>
     </row>

</xml_diff>

<commit_message>
Update BOM status and add an invoice
</commit_message>
<xml_diff>
--- a/BOM_STS1_Sidepanels.xlsx
+++ b/BOM_STS1_Sidepanels.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="5"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="X+" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="533" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="525" uniqueCount="131">
   <si>
     <t>ID</t>
   </si>
@@ -237,9 +237,6 @@
     <t>Count</t>
   </si>
   <si>
-    <t>im HQ</t>
-  </si>
-  <si>
     <t>22u 10V</t>
   </si>
   <si>
@@ -279,9 +276,6 @@
     <t>R21,R31,R41,R71</t>
   </si>
   <si>
-    <t>Digikey</t>
-  </si>
-  <si>
     <t>GUVA_Sensoren_Digikey.pdf</t>
   </si>
   <si>
@@ -366,9 +360,6 @@
     <t>YAGEO 10V 1uF X7R 0603 5% / Kondensator aus mehreren Keramikschichten MLCC - S</t>
   </si>
   <si>
-    <t>xx</t>
-  </si>
-  <si>
     <t>Samtec Zero Insertion Force / FFC &amp; FPC-Steckverbinder</t>
   </si>
   <si>
@@ -409,6 +400,18 @@
   </si>
   <si>
     <t>MELF Widerstände MELF Widerstände 1/4watt 22ohms 1% 50ppm 13</t>
+  </si>
+  <si>
+    <t>DK_INVOICE_106875107.pdf</t>
+  </si>
+  <si>
+    <t>/</t>
+  </si>
+  <si>
+    <t>Space Team assembles it</t>
+  </si>
+  <si>
+    <t>Note</t>
   </si>
 </sst>
 </file>
@@ -419,7 +422,7 @@
     <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
     <numFmt numFmtId="165" formatCode="#,##0.000\ &quot;€&quot;"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -448,8 +451,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -471,8 +482,13 @@
         <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -480,14 +496,30 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
@@ -500,8 +532,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="4"/>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="5">
+    <cellStyle name="Ausgabe" xfId="4" builtinId="21"/>
     <cellStyle name="Gut" xfId="1" builtinId="26"/>
     <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Schlecht" xfId="2" builtinId="27"/>
@@ -807,7 +841,7 @@
   <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -836,6 +870,9 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
+      <c r="G1" t="s">
+        <v>130</v>
+      </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
@@ -860,7 +897,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C3" t="s">
         <v>8</v>
@@ -869,11 +906,11 @@
         <v>2</v>
       </c>
       <c r="E3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F3" s="1"/>
       <c r="H3" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -881,7 +918,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C4" t="s">
         <v>8</v>
@@ -890,11 +927,11 @@
         <v>4</v>
       </c>
       <c r="E4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F4" s="1"/>
       <c r="H4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -915,7 +952,7 @@
       </c>
       <c r="F5" s="1"/>
       <c r="H5" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -934,7 +971,10 @@
       <c r="E6" t="s">
         <v>14</v>
       </c>
-      <c r="F6" s="1"/>
+      <c r="F6" s="3"/>
+      <c r="G6" t="s">
+        <v>129</v>
+      </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
@@ -954,7 +994,7 @@
       </c>
       <c r="F7" s="1"/>
       <c r="H7" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -975,7 +1015,7 @@
       </c>
       <c r="F8" s="1"/>
       <c r="H8" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -983,7 +1023,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C9" t="s">
         <v>20</v>
@@ -996,7 +1036,7 @@
       </c>
       <c r="F9" s="1"/>
       <c r="H9" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -1017,7 +1057,7 @@
       </c>
       <c r="F10" s="1"/>
       <c r="H10" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -1025,7 +1065,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C11" t="s">
         <v>20</v>
@@ -1038,7 +1078,7 @@
       </c>
       <c r="F11" s="1"/>
       <c r="H11" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -1059,7 +1099,7 @@
       </c>
       <c r="F12" s="1"/>
       <c r="H12" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -1067,7 +1107,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C13" t="s">
         <v>28</v>
@@ -1080,7 +1120,7 @@
       </c>
       <c r="F13" s="1"/>
       <c r="H13" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -1101,7 +1141,7 @@
       </c>
       <c r="F14" s="1"/>
       <c r="H14" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -1109,7 +1149,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C15" t="s">
         <v>31</v>
@@ -1122,7 +1162,7 @@
       </c>
       <c r="F15" s="1"/>
       <c r="H15" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -1130,7 +1170,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C16" t="s">
         <v>31</v>
@@ -1143,7 +1183,7 @@
       </c>
       <c r="F16" s="1"/>
       <c r="H16" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -1164,7 +1204,7 @@
       </c>
       <c r="F17" s="1"/>
       <c r="H17" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -1183,12 +1223,9 @@
       <c r="E18" t="s">
         <v>39</v>
       </c>
-      <c r="F18" s="2"/>
-      <c r="G18" t="s">
-        <v>86</v>
-      </c>
+      <c r="F18" s="1"/>
       <c r="H18" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>
@@ -1201,7 +1238,7 @@
   <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1248,11 +1285,8 @@
         <v>42</v>
       </c>
       <c r="F2" s="3"/>
-      <c r="G2" t="s">
-        <v>72</v>
-      </c>
       <c r="H2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -1273,7 +1307,7 @@
       </c>
       <c r="F3" s="1"/>
       <c r="H3" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -1281,7 +1315,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C4" t="s">
         <v>31</v>
@@ -1294,7 +1328,7 @@
       </c>
       <c r="F4" s="1"/>
       <c r="H4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -1313,12 +1347,9 @@
       <c r="E5" t="s">
         <v>39</v>
       </c>
-      <c r="F5" s="2"/>
-      <c r="G5" t="s">
-        <v>86</v>
-      </c>
+      <c r="F5" s="1"/>
       <c r="H5" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -1326,7 +1357,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C6" t="s">
         <v>8</v>
@@ -1335,11 +1366,11 @@
         <v>2</v>
       </c>
       <c r="E6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F6" s="1"/>
       <c r="H6" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -1347,7 +1378,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C7" t="s">
         <v>8</v>
@@ -1356,11 +1387,11 @@
         <v>4</v>
       </c>
       <c r="E7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F7" s="1"/>
       <c r="H7" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -1381,7 +1412,7 @@
       </c>
       <c r="F8" s="1"/>
       <c r="H8" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -1402,7 +1433,7 @@
       </c>
       <c r="F9" s="1"/>
       <c r="H9" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -1423,7 +1454,7 @@
       </c>
       <c r="F10" s="1"/>
       <c r="H10" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -1444,7 +1475,7 @@
       </c>
       <c r="F11" s="1"/>
       <c r="H11" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -1452,7 +1483,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C12" t="s">
         <v>20</v>
@@ -1465,7 +1496,7 @@
       </c>
       <c r="F12" s="1"/>
       <c r="H12" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -1473,7 +1504,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C13" t="s">
         <v>20</v>
@@ -1486,7 +1517,7 @@
       </c>
       <c r="F13" s="1"/>
       <c r="H13" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -1507,7 +1538,7 @@
       </c>
       <c r="F14" s="1"/>
       <c r="H14" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -1515,7 +1546,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C15" t="s">
         <v>28</v>
@@ -1528,7 +1559,7 @@
       </c>
       <c r="F15" s="1"/>
       <c r="H15" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -1536,7 +1567,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C16" t="s">
         <v>31</v>
@@ -1549,7 +1580,7 @@
       </c>
       <c r="F16" s="1"/>
       <c r="H16" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -1570,7 +1601,7 @@
       </c>
       <c r="F17" s="1"/>
       <c r="H17" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -1591,7 +1622,7 @@
       </c>
       <c r="F18" s="1"/>
       <c r="H18" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -1612,7 +1643,7 @@
       </c>
       <c r="F19" s="1"/>
       <c r="H19" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -1633,7 +1664,7 @@
       </c>
       <c r="F20" s="1"/>
       <c r="H20" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -1646,7 +1677,7 @@
   <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1693,11 +1724,8 @@
         <v>42</v>
       </c>
       <c r="F2" s="3"/>
-      <c r="G2" t="s">
-        <v>72</v>
-      </c>
       <c r="H2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -1718,7 +1746,7 @@
       </c>
       <c r="F3" s="1"/>
       <c r="H3" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -1726,7 +1754,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C4" t="s">
         <v>31</v>
@@ -1739,7 +1767,7 @@
       </c>
       <c r="F4" s="1"/>
       <c r="H4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -1758,12 +1786,9 @@
       <c r="E5" t="s">
         <v>39</v>
       </c>
-      <c r="F5" s="2"/>
-      <c r="G5" t="s">
-        <v>86</v>
-      </c>
+      <c r="F5" s="1"/>
       <c r="H5" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -1771,7 +1796,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C6" t="s">
         <v>8</v>
@@ -1780,11 +1805,11 @@
         <v>2</v>
       </c>
       <c r="E6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F6" s="1"/>
       <c r="H6" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -1792,7 +1817,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C7" t="s">
         <v>8</v>
@@ -1801,11 +1826,11 @@
         <v>4</v>
       </c>
       <c r="E7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F7" s="1"/>
       <c r="H7" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -1826,7 +1851,7 @@
       </c>
       <c r="F8" s="1"/>
       <c r="H8" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -1847,7 +1872,7 @@
       </c>
       <c r="F9" s="1"/>
       <c r="H9" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -1868,7 +1893,7 @@
       </c>
       <c r="F10" s="1"/>
       <c r="H10" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -1889,7 +1914,7 @@
       </c>
       <c r="F11" s="1"/>
       <c r="H11" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -1897,7 +1922,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C12" t="s">
         <v>20</v>
@@ -1910,7 +1935,7 @@
       </c>
       <c r="F12" s="1"/>
       <c r="H12" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -1918,7 +1943,7 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C13" t="s">
         <v>20</v>
@@ -1931,7 +1956,7 @@
       </c>
       <c r="F13" s="1"/>
       <c r="H13" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -1952,7 +1977,7 @@
       </c>
       <c r="F14" s="1"/>
       <c r="H14" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -1960,7 +1985,7 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C15" t="s">
         <v>28</v>
@@ -1973,7 +1998,7 @@
       </c>
       <c r="F15" s="1"/>
       <c r="H15" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -1981,7 +2006,7 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C16" t="s">
         <v>31</v>
@@ -1994,7 +2019,7 @@
       </c>
       <c r="F16" s="1"/>
       <c r="H16" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -2015,7 +2040,7 @@
       </c>
       <c r="F17" s="1"/>
       <c r="H17" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -2036,7 +2061,7 @@
       </c>
       <c r="F18" s="1"/>
       <c r="H18" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -2057,7 +2082,7 @@
       </c>
       <c r="F19" s="1"/>
       <c r="H19" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -2078,7 +2103,7 @@
       </c>
       <c r="F20" s="1"/>
       <c r="H20" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -2090,8 +2115,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14:E14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2138,11 +2163,8 @@
         <v>42</v>
       </c>
       <c r="F2" s="3"/>
-      <c r="G2" t="s">
-        <v>72</v>
-      </c>
       <c r="H2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -2161,12 +2183,9 @@
       <c r="E3" t="s">
         <v>58</v>
       </c>
-      <c r="F3" s="2"/>
-      <c r="G3" t="s">
-        <v>86</v>
-      </c>
+      <c r="F3" s="1"/>
       <c r="H3" t="s">
-        <v>92</v>
+        <v>127</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -2174,7 +2193,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C4" t="s">
         <v>20</v>
@@ -2187,7 +2206,7 @@
       </c>
       <c r="F4" s="1"/>
       <c r="H4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -2208,7 +2227,7 @@
       </c>
       <c r="F5" s="1"/>
       <c r="H5" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -2229,7 +2248,7 @@
       </c>
       <c r="F6" s="1"/>
       <c r="H6" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -2250,7 +2269,7 @@
       </c>
       <c r="F7" s="1"/>
       <c r="H7" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -2271,7 +2290,7 @@
       </c>
       <c r="F8" s="1"/>
       <c r="H8" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -2279,7 +2298,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C9" t="s">
         <v>8</v>
@@ -2288,11 +2307,11 @@
         <v>1</v>
       </c>
       <c r="E9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F9" s="1"/>
       <c r="H9" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -2300,7 +2319,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C10" t="s">
         <v>8</v>
@@ -2309,11 +2328,11 @@
         <v>2</v>
       </c>
       <c r="E10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F10" s="1"/>
       <c r="H10" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -2334,7 +2353,7 @@
       </c>
       <c r="F11" s="1"/>
       <c r="H11" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -2355,7 +2374,7 @@
       </c>
       <c r="F12" s="1"/>
       <c r="H12" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -2374,12 +2393,9 @@
       <c r="E13" t="s">
         <v>39</v>
       </c>
-      <c r="F13" s="2"/>
-      <c r="G13" t="s">
-        <v>86</v>
-      </c>
+      <c r="F13" s="1"/>
       <c r="H13" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -2400,7 +2416,7 @@
       </c>
       <c r="F14" s="1"/>
       <c r="H14" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -2421,7 +2437,7 @@
       </c>
       <c r="F15" s="1"/>
       <c r="H15" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -2442,7 +2458,7 @@
       </c>
       <c r="F16" s="1"/>
       <c r="H16" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -2463,7 +2479,7 @@
       </c>
       <c r="F17" s="1"/>
       <c r="H17" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -2484,7 +2500,7 @@
       </c>
       <c r="F18" s="1"/>
       <c r="H18" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -2505,7 +2521,7 @@
       </c>
       <c r="F19" s="1"/>
       <c r="H19" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -2526,7 +2542,7 @@
       </c>
       <c r="F20" s="1"/>
       <c r="H20" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
@@ -2547,7 +2563,7 @@
       </c>
       <c r="F21" s="1"/>
       <c r="H21" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -2560,7 +2576,7 @@
   <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2592,7 +2608,7 @@
         <v>4</v>
       </c>
       <c r="H1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -2612,11 +2628,8 @@
         <v>42</v>
       </c>
       <c r="F2" s="3"/>
-      <c r="G2" t="s">
-        <v>72</v>
-      </c>
       <c r="H2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -2637,7 +2650,7 @@
       </c>
       <c r="F3" s="1"/>
       <c r="H3" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -2658,7 +2671,7 @@
       </c>
       <c r="F4" s="1"/>
       <c r="H4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -2679,7 +2692,7 @@
       </c>
       <c r="F5" s="1"/>
       <c r="H5" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -2700,7 +2713,7 @@
       </c>
       <c r="F6" s="1"/>
       <c r="H6" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -2721,7 +2734,7 @@
       </c>
       <c r="F7" s="1"/>
       <c r="H7" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -2742,7 +2755,7 @@
       </c>
       <c r="F8" s="1"/>
       <c r="H8" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -2763,7 +2776,7 @@
       </c>
       <c r="F9" s="1"/>
       <c r="H9" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -2771,7 +2784,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C10" t="s">
         <v>20</v>
@@ -2784,7 +2797,7 @@
       </c>
       <c r="F10" s="1"/>
       <c r="H10" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -2803,12 +2816,9 @@
       <c r="E11" t="s">
         <v>39</v>
       </c>
-      <c r="F11" s="2"/>
-      <c r="G11" t="s">
-        <v>86</v>
-      </c>
+      <c r="F11" s="1"/>
       <c r="H11" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -2829,7 +2839,7 @@
       </c>
       <c r="F12" s="1"/>
       <c r="H12" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -2850,7 +2860,7 @@
       </c>
       <c r="F13" s="1"/>
       <c r="H13" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -2871,7 +2881,7 @@
       </c>
       <c r="F14" s="1"/>
       <c r="H14" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -2890,12 +2900,9 @@
       <c r="E15" t="s">
         <v>58</v>
       </c>
-      <c r="F15" s="2"/>
-      <c r="G15" t="s">
-        <v>86</v>
-      </c>
+      <c r="F15" s="1"/>
       <c r="H15" t="s">
-        <v>92</v>
+        <v>127</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -2916,7 +2923,7 @@
       </c>
       <c r="F16" s="1"/>
       <c r="H16" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -2924,7 +2931,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C17" t="s">
         <v>8</v>
@@ -2933,11 +2940,11 @@
         <v>1</v>
       </c>
       <c r="E17" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F17" s="1"/>
       <c r="H17" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -2945,7 +2952,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C18" t="s">
         <v>8</v>
@@ -2954,11 +2961,11 @@
         <v>2</v>
       </c>
       <c r="E18" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F18" s="1"/>
       <c r="H18" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -2979,7 +2986,7 @@
       </c>
       <c r="F19" s="1"/>
       <c r="H19" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -3000,7 +3007,7 @@
       </c>
       <c r="F20" s="1"/>
       <c r="H20" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
@@ -3021,7 +3028,7 @@
       </c>
       <c r="F21" s="1"/>
       <c r="H21" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -3031,824 +3038,759 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J35"/>
+  <dimension ref="A1:I34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="32.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="89" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="89" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
+        <v>91</v>
+      </c>
+      <c r="E1" t="s">
+        <v>92</v>
+      </c>
+      <c r="F1" t="s">
+        <v>93</v>
+      </c>
+      <c r="G1" t="s">
+        <v>98</v>
+      </c>
+      <c r="H1" t="s">
+        <v>119</v>
+      </c>
+      <c r="I1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="2"/>
+      <c r="C2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D2" t="s">
+        <v>85</v>
+      </c>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6">
+        <f>H2*B2</f>
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>71</v>
-      </c>
-      <c r="D1" t="s">
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="B3">
+        <v>24</v>
+      </c>
+      <c r="C3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D3" t="s">
+        <v>86</v>
+      </c>
+      <c r="E3">
+        <v>8532240000</v>
+      </c>
+      <c r="F3" t="s">
+        <v>112</v>
+      </c>
+      <c r="G3" t="s">
+        <v>109</v>
+      </c>
+      <c r="H3" s="6">
+        <v>9.1999999999999998E-2</v>
+      </c>
+      <c r="I3" s="6">
+        <f t="shared" ref="I3:I21" si="0">H3*B3</f>
+        <v>2.2080000000000002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="B4">
         <v>4</v>
       </c>
-      <c r="E1" t="s">
-        <v>93</v>
-      </c>
-      <c r="F1" t="s">
-        <v>94</v>
-      </c>
-      <c r="G1" t="s">
-        <v>95</v>
-      </c>
-      <c r="H1" t="s">
-        <v>100</v>
-      </c>
-      <c r="I1" t="s">
+      <c r="C4" t="s">
+        <v>56</v>
+      </c>
+      <c r="D4" t="s">
+        <v>86</v>
+      </c>
+      <c r="E4">
+        <v>8542399000</v>
+      </c>
+      <c r="F4" t="s">
         <v>122</v>
       </c>
-      <c r="J1" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C2" s="2"/>
-      <c r="D2" t="s">
-        <v>42</v>
-      </c>
-      <c r="E2" t="s">
-        <v>87</v>
-      </c>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6">
-        <f>I2*C2</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C3">
-        <v>24</v>
-      </c>
-      <c r="D3" t="s">
-        <v>33</v>
-      </c>
-      <c r="E3" t="s">
-        <v>88</v>
-      </c>
-      <c r="F3">
-        <v>8532240000</v>
-      </c>
-      <c r="G3" t="s">
-        <v>114</v>
-      </c>
-      <c r="H3" t="s">
-        <v>111</v>
-      </c>
-      <c r="I3" s="6">
-        <v>9.1999999999999998E-2</v>
-      </c>
-      <c r="J3" s="6">
-        <f t="shared" ref="J3:J35" si="0">I3*C3</f>
-        <v>2.2080000000000002</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>54</v>
-      </c>
-      <c r="C4">
-        <v>4</v>
-      </c>
-      <c r="D4" t="s">
-        <v>56</v>
-      </c>
-      <c r="E4" t="s">
-        <v>88</v>
-      </c>
-      <c r="F4">
-        <v>8542399000</v>
-      </c>
       <c r="G4" t="s">
-        <v>125</v>
-      </c>
-      <c r="H4" t="s">
-        <v>126</v>
+        <v>123</v>
+      </c>
+      <c r="H4" s="6">
+        <v>2.44</v>
       </c>
       <c r="I4" s="6">
-        <v>2.44</v>
-      </c>
-      <c r="J4" s="6">
         <f t="shared" si="0"/>
         <v>9.76</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="C5">
+      <c r="B5">
         <v>32</v>
       </c>
+      <c r="C5" t="s">
+        <v>32</v>
+      </c>
       <c r="D5" t="s">
-        <v>32</v>
-      </c>
-      <c r="E5" t="s">
-        <v>88</v>
-      </c>
-      <c r="F5">
+        <v>86</v>
+      </c>
+      <c r="E5">
         <v>8532240000</v>
       </c>
+      <c r="F5" t="s">
+        <v>111</v>
+      </c>
       <c r="G5" t="s">
-        <v>113</v>
-      </c>
-      <c r="H5" t="s">
-        <v>111</v>
+        <v>109</v>
+      </c>
+      <c r="H5" s="6">
+        <v>3.7999999999999999E-2</v>
       </c>
       <c r="I5" s="6">
-        <v>3.7999999999999999E-2</v>
-      </c>
-      <c r="J5" s="6">
         <f t="shared" si="0"/>
         <v>1.216</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="C6">
+      <c r="B6">
         <v>13</v>
       </c>
+      <c r="C6" t="s">
+        <v>19</v>
+      </c>
       <c r="D6" t="s">
-        <v>19</v>
-      </c>
-      <c r="E6" t="s">
-        <v>90</v>
-      </c>
-      <c r="F6">
+        <v>88</v>
+      </c>
+      <c r="E6">
         <v>85423990</v>
       </c>
+      <c r="F6" t="s">
+        <v>120</v>
+      </c>
       <c r="G6" t="s">
-        <v>123</v>
-      </c>
-      <c r="H6" t="s">
-        <v>124</v>
+        <v>121</v>
+      </c>
+      <c r="H6" s="6">
+        <v>3.91</v>
       </c>
       <c r="I6" s="6">
-        <v>3.91</v>
-      </c>
-      <c r="J6" s="6">
         <f t="shared" si="0"/>
         <v>50.83</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="C7">
+      <c r="B7">
         <v>16</v>
       </c>
+      <c r="C7" t="s">
+        <v>17</v>
+      </c>
       <c r="D7" t="s">
-        <v>17</v>
-      </c>
-      <c r="E7" t="s">
-        <v>88</v>
-      </c>
-      <c r="F7">
+        <v>86</v>
+      </c>
+      <c r="E7">
         <v>8541100000</v>
       </c>
+      <c r="F7" t="s">
+        <v>115</v>
+      </c>
       <c r="G7" t="s">
-        <v>118</v>
-      </c>
-      <c r="H7" t="s">
-        <v>101</v>
+        <v>99</v>
+      </c>
+      <c r="H7" s="6">
+        <v>0.46500000000000002</v>
       </c>
       <c r="I7" s="6">
-        <v>0.46500000000000002</v>
-      </c>
-      <c r="J7" s="6">
         <f t="shared" si="0"/>
         <v>7.44</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="C8">
+      <c r="B8">
         <v>16</v>
       </c>
+      <c r="C8" t="s">
+        <v>30</v>
+      </c>
       <c r="D8" t="s">
-        <v>30</v>
-      </c>
-      <c r="E8" t="s">
-        <v>88</v>
-      </c>
-      <c r="F8">
+        <v>86</v>
+      </c>
+      <c r="E8">
         <v>8533210000</v>
       </c>
+      <c r="F8" t="s">
+        <v>110</v>
+      </c>
       <c r="G8" t="s">
-        <v>112</v>
-      </c>
-      <c r="H8" t="s">
-        <v>111</v>
+        <v>109</v>
+      </c>
+      <c r="H8" s="6">
+        <v>0.28100000000000003</v>
       </c>
       <c r="I8" s="6">
-        <v>0.28100000000000003</v>
-      </c>
-      <c r="J8" s="6">
         <f t="shared" si="0"/>
         <v>4.4960000000000004</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C9">
+      <c r="B9">
         <v>16</v>
       </c>
+      <c r="C9" t="s">
+        <v>25</v>
+      </c>
       <c r="D9" t="s">
-        <v>25</v>
-      </c>
-      <c r="E9" t="s">
-        <v>88</v>
-      </c>
-      <c r="F9">
+        <v>86</v>
+      </c>
+      <c r="E9">
         <v>8533210000</v>
       </c>
+      <c r="F9" t="s">
+        <v>102</v>
+      </c>
       <c r="G9" t="s">
-        <v>104</v>
-      </c>
-      <c r="H9" t="s">
-        <v>103</v>
+        <v>101</v>
+      </c>
+      <c r="H9" s="6">
+        <v>0.222</v>
       </c>
       <c r="I9" s="6">
-        <v>0.222</v>
-      </c>
-      <c r="J9" s="6">
         <f t="shared" si="0"/>
         <v>3.552</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
-        <v>85</v>
-      </c>
-      <c r="C10">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="B10">
         <v>48</v>
       </c>
+      <c r="C10" t="s">
+        <v>21</v>
+      </c>
       <c r="D10" t="s">
-        <v>21</v>
-      </c>
-      <c r="E10" t="s">
-        <v>88</v>
-      </c>
-      <c r="F10">
+        <v>86</v>
+      </c>
+      <c r="E10">
         <v>8533210000</v>
       </c>
+      <c r="F10" t="s">
+        <v>105</v>
+      </c>
       <c r="G10" t="s">
-        <v>107</v>
-      </c>
-      <c r="H10" t="s">
-        <v>102</v>
+        <v>100</v>
+      </c>
+      <c r="H10" s="6">
+        <v>0.20300000000000001</v>
       </c>
       <c r="I10" s="6">
-        <v>0.20300000000000001</v>
-      </c>
-      <c r="J10" s="6">
         <f t="shared" si="0"/>
         <v>9.7439999999999998</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="C11">
+      <c r="B11">
         <v>12</v>
       </c>
+      <c r="C11" t="s">
+        <v>39</v>
+      </c>
       <c r="D11" t="s">
-        <v>39</v>
-      </c>
-      <c r="E11" t="s">
-        <v>91</v>
-      </c>
-      <c r="F11">
+        <v>89</v>
+      </c>
+      <c r="E11">
         <v>8504508000</v>
       </c>
+      <c r="F11" t="s">
+        <v>94</v>
+      </c>
       <c r="G11" t="s">
-        <v>96</v>
+        <v>128</v>
+      </c>
+      <c r="H11" s="6">
+        <v>3.3</v>
       </c>
       <c r="I11" s="6">
-        <v>3.3</v>
-      </c>
-      <c r="J11" s="6">
         <f t="shared" si="0"/>
         <v>39.599999999999994</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>11</v>
-      </c>
-      <c r="B12" t="s">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="C12">
+      <c r="B12">
         <v>50</v>
       </c>
+      <c r="C12" t="s">
+        <v>46</v>
+      </c>
       <c r="D12" t="s">
-        <v>46</v>
-      </c>
-      <c r="E12" t="s">
-        <v>89</v>
-      </c>
-      <c r="F12">
+        <v>87</v>
+      </c>
+      <c r="E12">
         <v>8533210000</v>
+      </c>
+      <c r="F12" t="s">
+        <v>97</v>
       </c>
       <c r="G12" t="s">
         <v>99</v>
       </c>
-      <c r="H12" t="s">
-        <v>101</v>
+      <c r="H12" s="6">
+        <v>1.7999999999999999E-2</v>
       </c>
       <c r="I12" s="6">
-        <v>1.7999999999999999E-2</v>
-      </c>
-      <c r="J12" s="6">
         <f t="shared" si="0"/>
         <v>0.89999999999999991</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>12</v>
-      </c>
-      <c r="B13" t="s">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="C13">
+      <c r="B13">
         <v>16</v>
       </c>
+      <c r="C13" t="s">
+        <v>27</v>
+      </c>
       <c r="D13" t="s">
-        <v>27</v>
-      </c>
-      <c r="E13" t="s">
-        <v>88</v>
-      </c>
-      <c r="F13">
+        <v>86</v>
+      </c>
+      <c r="E13">
         <v>8533210000</v>
       </c>
+      <c r="F13" t="s">
+        <v>107</v>
+      </c>
       <c r="G13" t="s">
-        <v>109</v>
-      </c>
-      <c r="H13" t="s">
-        <v>102</v>
+        <v>100</v>
+      </c>
+      <c r="H13" s="6">
+        <v>0.29599999999999999</v>
       </c>
       <c r="I13" s="6">
-        <v>0.29599999999999999</v>
-      </c>
-      <c r="J13" s="6">
         <f t="shared" si="0"/>
         <v>4.7359999999999998</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>13</v>
-      </c>
-      <c r="B14" t="s">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="C14">
+      <c r="B14">
         <v>6</v>
       </c>
+      <c r="C14" t="s">
+        <v>43</v>
+      </c>
       <c r="D14" t="s">
-        <v>43</v>
-      </c>
-      <c r="E14" t="s">
-        <v>88</v>
-      </c>
-      <c r="F14">
+        <v>86</v>
+      </c>
+      <c r="E14">
         <v>8536693000</v>
       </c>
+      <c r="F14" t="s">
+        <v>113</v>
+      </c>
       <c r="G14" t="s">
-        <v>116</v>
-      </c>
-      <c r="H14" t="s">
-        <v>117</v>
+        <v>114</v>
+      </c>
+      <c r="H14" s="6">
+        <v>2.16</v>
       </c>
       <c r="I14" s="6">
-        <v>2.16</v>
-      </c>
-      <c r="J14" s="6">
         <f t="shared" si="0"/>
         <v>12.96</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>14</v>
-      </c>
-      <c r="B15" t="s">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="C15">
+      <c r="B15">
         <v>10</v>
       </c>
+      <c r="C15" t="s">
+        <v>58</v>
+      </c>
       <c r="D15" t="s">
-        <v>58</v>
-      </c>
-      <c r="E15" t="s">
-        <v>92</v>
-      </c>
-      <c r="F15">
+        <v>90</v>
+      </c>
+      <c r="E15">
         <v>8536694051</v>
       </c>
+      <c r="F15" t="s">
+        <v>95</v>
+      </c>
       <c r="G15" t="s">
-        <v>97</v>
-      </c>
-      <c r="H15" t="s">
-        <v>101</v>
+        <v>99</v>
+      </c>
+      <c r="H15" s="6">
+        <v>2.1230000000000002</v>
       </c>
       <c r="I15" s="6">
-        <v>2.1230000000000002</v>
-      </c>
-      <c r="J15" s="6">
         <f t="shared" si="0"/>
         <v>21.230000000000004</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>15</v>
-      </c>
-      <c r="B16" t="s">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="C16">
+      <c r="B16">
         <v>6</v>
       </c>
+      <c r="C16" t="s">
+        <v>51</v>
+      </c>
       <c r="D16" t="s">
-        <v>51</v>
-      </c>
-      <c r="E16" t="s">
-        <v>88</v>
-      </c>
-      <c r="F16">
+        <v>86</v>
+      </c>
+      <c r="E16">
         <v>8536693000</v>
       </c>
+      <c r="F16" t="s">
+        <v>117</v>
+      </c>
       <c r="G16" t="s">
-        <v>120</v>
-      </c>
-      <c r="H16" t="s">
-        <v>121</v>
+        <v>118</v>
+      </c>
+      <c r="H16" s="6">
+        <v>0.49299999999999999</v>
       </c>
       <c r="I16" s="6">
-        <v>0.49299999999999999</v>
-      </c>
-      <c r="J16" s="6">
         <f t="shared" si="0"/>
         <v>2.9580000000000002</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>16</v>
-      </c>
-      <c r="B17" t="s">
-        <v>81</v>
-      </c>
-      <c r="C17">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="B17">
         <v>10</v>
       </c>
+      <c r="C17" t="s">
+        <v>72</v>
+      </c>
       <c r="D17" t="s">
-        <v>73</v>
-      </c>
-      <c r="E17" t="s">
-        <v>88</v>
-      </c>
-      <c r="F17">
+        <v>86</v>
+      </c>
+      <c r="E17">
         <v>8532210000</v>
       </c>
+      <c r="F17" t="s">
+        <v>104</v>
+      </c>
       <c r="G17" t="s">
-        <v>106</v>
-      </c>
-      <c r="H17" t="s">
-        <v>105</v>
+        <v>103</v>
+      </c>
+      <c r="H17" s="6">
+        <v>2.41</v>
       </c>
       <c r="I17" s="6">
-        <v>2.41</v>
-      </c>
-      <c r="J17" s="6">
         <f t="shared" si="0"/>
         <v>24.1</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>17</v>
-      </c>
-      <c r="B18" t="s">
-        <v>80</v>
-      </c>
-      <c r="C18">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="B18">
         <v>32</v>
       </c>
+      <c r="C18" t="s">
+        <v>73</v>
+      </c>
       <c r="D18" t="s">
-        <v>74</v>
-      </c>
-      <c r="E18" t="s">
-        <v>88</v>
-      </c>
-      <c r="F18">
+        <v>86</v>
+      </c>
+      <c r="E18">
         <v>8532240000</v>
       </c>
+      <c r="F18" t="s">
+        <v>96</v>
+      </c>
       <c r="G18" t="s">
-        <v>98</v>
-      </c>
-      <c r="H18" t="s">
-        <v>102</v>
+        <v>100</v>
+      </c>
+      <c r="H18" s="6">
+        <v>0.27100000000000002</v>
       </c>
       <c r="I18" s="6">
-        <v>0.27100000000000002</v>
-      </c>
-      <c r="J18" s="6">
         <f t="shared" si="0"/>
         <v>8.6720000000000006</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>18</v>
-      </c>
-      <c r="B19" t="s">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C19">
+      <c r="B19">
         <v>6</v>
       </c>
+      <c r="C19" t="s">
+        <v>11</v>
+      </c>
       <c r="D19" t="s">
-        <v>11</v>
-      </c>
-      <c r="E19" t="s">
-        <v>88</v>
-      </c>
-      <c r="F19">
+        <v>86</v>
+      </c>
+      <c r="E19">
         <v>8533401000</v>
       </c>
+      <c r="F19" t="s">
+        <v>116</v>
+      </c>
       <c r="G19" t="s">
-        <v>119</v>
-      </c>
-      <c r="H19" t="s">
-        <v>102</v>
+        <v>100</v>
+      </c>
+      <c r="H19" s="6">
+        <v>0.53900000000000003</v>
       </c>
       <c r="I19" s="6">
-        <v>0.53900000000000003</v>
-      </c>
-      <c r="J19" s="6">
         <f t="shared" si="0"/>
         <v>3.234</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>19</v>
-      </c>
-      <c r="B20" t="s">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="C20">
+      <c r="B20">
         <v>16</v>
       </c>
+      <c r="C20" t="s">
+        <v>29</v>
+      </c>
       <c r="D20" t="s">
-        <v>29</v>
-      </c>
-      <c r="E20" t="s">
-        <v>88</v>
-      </c>
-      <c r="F20">
+        <v>86</v>
+      </c>
+      <c r="E20">
         <v>8542330001</v>
       </c>
+      <c r="F20" t="s">
+        <v>108</v>
+      </c>
       <c r="G20" t="s">
-        <v>110</v>
-      </c>
-      <c r="H20" t="s">
-        <v>101</v>
+        <v>99</v>
+      </c>
+      <c r="H20" s="6">
+        <v>0.55300000000000005</v>
       </c>
       <c r="I20" s="6">
-        <v>0.55300000000000005</v>
-      </c>
-      <c r="J20" s="6">
         <f t="shared" si="0"/>
         <v>8.8480000000000008</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>20</v>
-      </c>
-      <c r="B21" t="s">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="C21">
+      <c r="B21">
         <v>16</v>
       </c>
+      <c r="C21" t="s">
+        <v>23</v>
+      </c>
       <c r="D21" t="s">
-        <v>23</v>
-      </c>
-      <c r="E21" t="s">
-        <v>88</v>
-      </c>
-      <c r="F21">
+        <v>86</v>
+      </c>
+      <c r="E21">
         <v>8541100000</v>
       </c>
+      <c r="F21" t="s">
+        <v>106</v>
+      </c>
       <c r="G21" t="s">
-        <v>108</v>
-      </c>
-      <c r="H21" t="s">
-        <v>101</v>
+        <v>99</v>
+      </c>
+      <c r="H21" s="6">
+        <v>0.254</v>
       </c>
       <c r="I21" s="6">
-        <v>0.254</v>
-      </c>
-      <c r="J21" s="6">
         <f t="shared" si="0"/>
         <v>4.0640000000000001</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="I22" s="6"/>
-      <c r="J22" s="6">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="I23" s="6"/>
-      <c r="J23" s="6">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>115</v>
-      </c>
-      <c r="B24" t="s">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="C24">
+      <c r="B22">
         <v>3</v>
       </c>
+      <c r="C22" t="s">
+        <v>63</v>
+      </c>
+      <c r="D22" t="s">
+        <v>86</v>
+      </c>
+      <c r="E22">
+        <v>8536693000</v>
+      </c>
+      <c r="F22" t="s">
+        <v>113</v>
+      </c>
+      <c r="G22" t="s">
+        <v>114</v>
+      </c>
+      <c r="H22" s="6">
+        <v>2.4500000000000002</v>
+      </c>
+      <c r="I22" s="6">
+        <f>H22*B22</f>
+        <v>7.3500000000000005</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B23">
+        <v>4</v>
+      </c>
+      <c r="C23" t="s">
+        <v>7</v>
+      </c>
+      <c r="D23" t="s">
+        <v>125</v>
+      </c>
+      <c r="E23">
+        <v>8533210000</v>
+      </c>
+      <c r="F23" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="G23" t="s">
+        <v>101</v>
+      </c>
+      <c r="H23" s="6">
+        <v>0.104</v>
+      </c>
+      <c r="I23" s="6">
+        <f>H23*B23</f>
+        <v>0.41599999999999998</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="B24">
+        <v>6</v>
+      </c>
+      <c r="C24" s="4">
+        <v>545482271</v>
+      </c>
       <c r="D24" t="s">
-        <v>63</v>
-      </c>
-      <c r="E24" t="s">
-        <v>88</v>
-      </c>
-      <c r="F24">
-        <v>8536693000</v>
+        <v>127</v>
+      </c>
+      <c r="E24">
+        <v>8536694051</v>
+      </c>
+      <c r="F24" t="s">
+        <v>95</v>
       </c>
       <c r="G24" t="s">
-        <v>116</v>
-      </c>
-      <c r="H24" t="s">
-        <v>117</v>
+        <v>99</v>
+      </c>
+      <c r="H24" s="6">
+        <v>2.35</v>
       </c>
       <c r="I24" s="6">
-        <v>2.4500000000000002</v>
-      </c>
-      <c r="J24" s="6">
-        <f t="shared" si="0"/>
-        <v>7.3500000000000005</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B25" t="s">
-        <v>12</v>
-      </c>
-      <c r="D25" t="s">
-        <v>13</v>
-      </c>
-      <c r="E25" s="2"/>
-      <c r="I25" s="6"/>
-      <c r="J25" s="6">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B26" t="s">
-        <v>5</v>
-      </c>
-      <c r="C26">
-        <v>4</v>
-      </c>
-      <c r="D26" t="s">
-        <v>7</v>
-      </c>
-      <c r="E26" t="s">
-        <v>128</v>
-      </c>
-      <c r="F26">
-        <v>8533210000</v>
-      </c>
-      <c r="G26" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="H26" t="s">
-        <v>103</v>
-      </c>
-      <c r="I26" s="6">
-        <v>0.104</v>
-      </c>
-      <c r="J26" s="6">
-        <f t="shared" si="0"/>
-        <v>0.41599999999999998</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+        <f>H24*B24</f>
+        <v>14.100000000000001</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H27" s="6"/>
       <c r="I27" s="6"/>
-      <c r="J27" s="6"/>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="I28" s="6"/>
-      <c r="J28" s="6"/>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H28" s="6"/>
+      <c r="I28" s="6">
+        <f>SUM(I2:I27)</f>
+        <v>242.41400000000002</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H29" s="6"/>
       <c r="I29" s="6"/>
-      <c r="J29" s="6">
-        <f>SUM(J2:J26)</f>
-        <v>228.31400000000002</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H30" s="6"/>
       <c r="I30" s="6"/>
-      <c r="J30" s="6"/>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H31" s="5"/>
       <c r="I31" s="6"/>
-      <c r="J31" s="6"/>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="I32" s="5"/>
-      <c r="J32" s="6"/>
-    </row>
-    <row r="33" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J33" s="6"/>
-    </row>
-    <row r="34" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J34" s="6"/>
-    </row>
-    <row r="35" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J35" s="6"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I32" s="6"/>
+    </row>
+    <row r="33" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I33" s="6"/>
+    </row>
+    <row r="34" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I34" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>